<commit_message>
More case handling edits
Corrected Concentration can now handle the case where a data set ends on an even chain instead of an odd chain. Average scaling factor will just use the scaling factor of the odd chain that comes before it.
</commit_message>
<xml_diff>
--- a/Ryan/GCData_for_Ryan_w_FaOH_STD_Data.xlsx
+++ b/Ryan/GCData_for_Ryan_w_FaOH_STD_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkong\Desktop\GitHub\GC_Code\Ryan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4666E1-63CA-4428-AD19-AB195F2399E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000405B4-A736-4398-9020-31846046AB67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="745" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="John_Code" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="59">
   <si>
     <t>PeakNo</t>
   </si>
@@ -655,7 +655,7 @@
   <dimension ref="A1:F1621"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35558,10 +35558,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F212"/>
+  <dimension ref="A1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37587,2222 +37587,2122 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102">
-        <v>11.526</v>
-      </c>
-      <c r="B102">
-        <v>11.494999999999999</v>
-      </c>
-      <c r="C102">
-        <v>11.592000000000001</v>
-      </c>
-      <c r="D102">
-        <v>3050</v>
-      </c>
-      <c r="E102">
-        <v>1924</v>
+      <c r="A102" t="s">
+        <v>20</v>
+      </c>
+      <c r="B102" t="s">
+        <v>20</v>
+      </c>
+      <c r="C102" t="s">
+        <v>20</v>
+      </c>
+      <c r="D102" t="s">
+        <v>20</v>
+      </c>
+      <c r="E102" t="s">
+        <v>20</v>
       </c>
       <c r="F102" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>11.513</v>
+        <v>3.4510000000000001</v>
       </c>
       <c r="B103">
-        <v>11.484999999999999</v>
+        <v>3.3650000000000002</v>
       </c>
       <c r="C103">
-        <v>11.593</v>
+        <v>3.6640000000000001</v>
       </c>
       <c r="D103">
-        <v>7476</v>
+        <v>153308</v>
       </c>
       <c r="E103">
-        <v>4518</v>
+        <v>36443</v>
       </c>
       <c r="F103" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>20</v>
-      </c>
-      <c r="B104" t="s">
-        <v>20</v>
-      </c>
-      <c r="C104" t="s">
-        <v>20</v>
-      </c>
-      <c r="D104" t="s">
-        <v>20</v>
-      </c>
-      <c r="E104" t="s">
-        <v>20</v>
+      <c r="A104">
+        <v>6.0049999999999999</v>
+      </c>
+      <c r="B104">
+        <v>5.9039999999999999</v>
+      </c>
+      <c r="C104">
+        <v>6.2489999999999997</v>
+      </c>
+      <c r="D104">
+        <v>188442</v>
+      </c>
+      <c r="E104">
+        <v>37250</v>
       </c>
       <c r="F104" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>3.4510000000000001</v>
+        <v>10.166</v>
       </c>
       <c r="B105">
-        <v>3.3650000000000002</v>
+        <v>10.038</v>
       </c>
       <c r="C105">
-        <v>3.6640000000000001</v>
+        <v>10.449</v>
       </c>
       <c r="D105">
-        <v>153308</v>
+        <v>199936</v>
       </c>
       <c r="E105">
-        <v>36443</v>
+        <v>49483</v>
       </c>
       <c r="F105" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>6.0049999999999999</v>
+        <v>12.439</v>
       </c>
       <c r="B106">
-        <v>5.9039999999999999</v>
+        <v>12.385999999999999</v>
       </c>
       <c r="C106">
-        <v>6.2489999999999997</v>
+        <v>12.61</v>
       </c>
       <c r="D106">
-        <v>188442</v>
+        <v>194893</v>
       </c>
       <c r="E106">
-        <v>37250</v>
+        <v>88230</v>
       </c>
       <c r="F106" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>10.166</v>
+        <v>13.861000000000001</v>
       </c>
       <c r="B107">
-        <v>10.038</v>
+        <v>13.808999999999999</v>
       </c>
       <c r="C107">
-        <v>10.449</v>
+        <v>13.972</v>
       </c>
       <c r="D107">
-        <v>199936</v>
+        <v>196024</v>
       </c>
       <c r="E107">
-        <v>49483</v>
+        <v>103060</v>
       </c>
       <c r="F107" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>12.439</v>
-      </c>
-      <c r="B108">
-        <v>12.385999999999999</v>
-      </c>
-      <c r="C108">
-        <v>12.61</v>
-      </c>
-      <c r="D108">
-        <v>194893</v>
-      </c>
-      <c r="E108">
-        <v>88230</v>
+      <c r="A108" t="s">
+        <v>21</v>
+      </c>
+      <c r="B108" t="s">
+        <v>21</v>
+      </c>
+      <c r="C108" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" t="s">
+        <v>21</v>
+      </c>
+      <c r="E108" t="s">
+        <v>21</v>
       </c>
       <c r="F108" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>13.861000000000001</v>
+        <v>3.4529999999999998</v>
       </c>
       <c r="B109">
-        <v>13.808999999999999</v>
+        <v>3.37</v>
       </c>
       <c r="C109">
-        <v>13.972</v>
+        <v>3.6680000000000001</v>
       </c>
       <c r="D109">
-        <v>196024</v>
+        <v>181600</v>
       </c>
       <c r="E109">
-        <v>103060</v>
+        <v>41801</v>
       </c>
       <c r="F109" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>21</v>
-      </c>
-      <c r="B110" t="s">
-        <v>21</v>
-      </c>
-      <c r="C110" t="s">
-        <v>21</v>
-      </c>
-      <c r="D110" t="s">
-        <v>21</v>
-      </c>
-      <c r="E110" t="s">
-        <v>21</v>
+      <c r="A110">
+        <v>4.67</v>
+      </c>
+      <c r="B110">
+        <v>4.6109999999999998</v>
+      </c>
+      <c r="C110">
+        <v>4.7050000000000001</v>
+      </c>
+      <c r="D110">
+        <v>552</v>
+      </c>
+      <c r="E110">
+        <v>164</v>
       </c>
       <c r="F110" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>3.4529999999999998</v>
+        <v>6.01</v>
       </c>
       <c r="B111">
-        <v>3.37</v>
+        <v>5.9089999999999998</v>
       </c>
       <c r="C111">
-        <v>3.6680000000000001</v>
+        <v>6.2539999999999996</v>
       </c>
       <c r="D111">
-        <v>181600</v>
+        <v>245715</v>
       </c>
       <c r="E111">
-        <v>41801</v>
+        <v>47622</v>
       </c>
       <c r="F111" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>4.67</v>
+        <v>10.17</v>
       </c>
       <c r="B112">
-        <v>4.6109999999999998</v>
+        <v>10.067</v>
       </c>
       <c r="C112">
-        <v>4.7050000000000001</v>
+        <v>10.462999999999999</v>
       </c>
       <c r="D112">
-        <v>552</v>
+        <v>264111</v>
       </c>
       <c r="E112">
-        <v>164</v>
+        <v>65143</v>
       </c>
       <c r="F112" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>6.01</v>
+        <v>12.441000000000001</v>
       </c>
       <c r="B113">
-        <v>5.9089999999999998</v>
+        <v>12.381</v>
       </c>
       <c r="C113">
-        <v>6.2539999999999996</v>
+        <v>12.61</v>
       </c>
       <c r="D113">
-        <v>245715</v>
+        <v>233669</v>
       </c>
       <c r="E113">
-        <v>47622</v>
+        <v>100998</v>
       </c>
       <c r="F113" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>10.17</v>
+        <v>13.861000000000001</v>
       </c>
       <c r="B114">
-        <v>10.067</v>
+        <v>13.814</v>
       </c>
       <c r="C114">
-        <v>10.462999999999999</v>
+        <v>13.949</v>
       </c>
       <c r="D114">
-        <v>264111</v>
+        <v>233107</v>
       </c>
       <c r="E114">
-        <v>65143</v>
+        <v>124026</v>
       </c>
       <c r="F114" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>12.441000000000001</v>
-      </c>
-      <c r="B115">
-        <v>12.381</v>
-      </c>
-      <c r="C115">
-        <v>12.61</v>
-      </c>
-      <c r="D115">
-        <v>233669</v>
-      </c>
-      <c r="E115">
-        <v>100998</v>
+      <c r="A115" t="s">
+        <v>22</v>
+      </c>
+      <c r="B115" t="s">
+        <v>22</v>
+      </c>
+      <c r="C115" t="s">
+        <v>22</v>
+      </c>
+      <c r="D115" t="s">
+        <v>22</v>
+      </c>
+      <c r="E115" t="s">
+        <v>22</v>
       </c>
       <c r="F115" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>13.861000000000001</v>
+        <v>3.4550000000000001</v>
       </c>
       <c r="B116">
-        <v>13.814</v>
+        <v>3.2949999999999999</v>
       </c>
       <c r="C116">
-        <v>13.949</v>
+        <v>3.673</v>
       </c>
       <c r="D116">
-        <v>233107</v>
+        <v>185483</v>
       </c>
       <c r="E116">
-        <v>124026</v>
+        <v>40901</v>
       </c>
       <c r="F116" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>22</v>
-      </c>
-      <c r="B117" t="s">
-        <v>22</v>
-      </c>
-      <c r="C117" t="s">
-        <v>22</v>
-      </c>
-      <c r="D117" t="s">
-        <v>22</v>
-      </c>
-      <c r="E117" t="s">
-        <v>22</v>
+      <c r="A117">
+        <v>4.6820000000000004</v>
+      </c>
+      <c r="B117">
+        <v>4.63</v>
+      </c>
+      <c r="C117">
+        <v>4.7320000000000002</v>
+      </c>
+      <c r="D117">
+        <v>690</v>
+      </c>
+      <c r="E117">
+        <v>166</v>
       </c>
       <c r="F117" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>3.4550000000000001</v>
+        <v>6.0140000000000002</v>
       </c>
       <c r="B118">
-        <v>3.2949999999999999</v>
+        <v>5.923</v>
       </c>
       <c r="C118">
-        <v>3.673</v>
+        <v>6.2309999999999999</v>
       </c>
       <c r="D118">
-        <v>185483</v>
+        <v>214835</v>
       </c>
       <c r="E118">
-        <v>40901</v>
+        <v>40625</v>
       </c>
       <c r="F118" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>4.6820000000000004</v>
+        <v>10.172000000000001</v>
       </c>
       <c r="B119">
-        <v>4.63</v>
+        <v>10.061999999999999</v>
       </c>
       <c r="C119">
-        <v>4.7320000000000002</v>
+        <v>10.481999999999999</v>
       </c>
       <c r="D119">
-        <v>690</v>
+        <v>214909</v>
       </c>
       <c r="E119">
-        <v>166</v>
+        <v>52070</v>
       </c>
       <c r="F119" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>6.0140000000000002</v>
+        <v>12.441000000000001</v>
       </c>
       <c r="B120">
-        <v>5.923</v>
+        <v>12.381</v>
       </c>
       <c r="C120">
-        <v>6.2309999999999999</v>
+        <v>12.615</v>
       </c>
       <c r="D120">
-        <v>214835</v>
+        <v>196608</v>
       </c>
       <c r="E120">
-        <v>40625</v>
+        <v>87761</v>
       </c>
       <c r="F120" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>10.172000000000001</v>
+        <v>13.86</v>
       </c>
       <c r="B121">
-        <v>10.061999999999999</v>
+        <v>13.814</v>
       </c>
       <c r="C121">
-        <v>10.481999999999999</v>
+        <v>13.962999999999999</v>
       </c>
       <c r="D121">
-        <v>214909</v>
+        <v>196562</v>
       </c>
       <c r="E121">
-        <v>52070</v>
+        <v>102781</v>
       </c>
       <c r="F121" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>12.441000000000001</v>
-      </c>
-      <c r="B122">
-        <v>12.381</v>
-      </c>
-      <c r="C122">
-        <v>12.615</v>
-      </c>
-      <c r="D122">
-        <v>196608</v>
-      </c>
-      <c r="E122">
-        <v>87761</v>
+      <c r="A122" t="s">
+        <v>23</v>
+      </c>
+      <c r="B122" t="s">
+        <v>23</v>
+      </c>
+      <c r="C122" t="s">
+        <v>23</v>
+      </c>
+      <c r="D122" t="s">
+        <v>23</v>
+      </c>
+      <c r="E122" t="s">
+        <v>23</v>
       </c>
       <c r="F122" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>13.86</v>
+        <v>3.456</v>
       </c>
       <c r="B123">
-        <v>13.814</v>
+        <v>3.3740000000000001</v>
       </c>
       <c r="C123">
-        <v>13.962999999999999</v>
+        <v>3.6819999999999999</v>
       </c>
       <c r="D123">
-        <v>196562</v>
+        <v>172506</v>
       </c>
       <c r="E123">
-        <v>102781</v>
+        <v>38428</v>
       </c>
       <c r="F123" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>23</v>
-      </c>
-      <c r="B124" t="s">
-        <v>23</v>
-      </c>
-      <c r="C124" t="s">
-        <v>23</v>
-      </c>
-      <c r="D124" t="s">
-        <v>23</v>
-      </c>
-      <c r="E124" t="s">
-        <v>23</v>
+      <c r="A124">
+        <v>4.577</v>
+      </c>
+      <c r="B124">
+        <v>4.4480000000000004</v>
+      </c>
+      <c r="C124">
+        <v>4.8070000000000004</v>
+      </c>
+      <c r="D124">
+        <v>194122</v>
+      </c>
+      <c r="E124">
+        <v>38514</v>
       </c>
       <c r="F124" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>3.456</v>
+        <v>6.0149999999999997</v>
       </c>
       <c r="B125">
-        <v>3.3740000000000001</v>
+        <v>5.9219999999999997</v>
       </c>
       <c r="C125">
-        <v>3.6819999999999999</v>
+        <v>6.2160000000000002</v>
       </c>
       <c r="D125">
-        <v>172506</v>
+        <v>212754</v>
       </c>
       <c r="E125">
-        <v>38428</v>
+        <v>39352</v>
       </c>
       <c r="F125" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>4.577</v>
+        <v>7.9370000000000003</v>
       </c>
       <c r="B126">
-        <v>4.4480000000000004</v>
+        <v>7.78</v>
       </c>
       <c r="C126">
-        <v>4.8070000000000004</v>
+        <v>8.4</v>
       </c>
       <c r="D126">
-        <v>194122</v>
+        <v>192177</v>
       </c>
       <c r="E126">
-        <v>38514</v>
+        <v>25962</v>
       </c>
       <c r="F126" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>6.0149999999999997</v>
+        <v>10.173</v>
       </c>
       <c r="B127">
-        <v>5.9219999999999997</v>
+        <v>10.071</v>
       </c>
       <c r="C127">
-        <v>6.2160000000000002</v>
+        <v>10.449</v>
       </c>
       <c r="D127">
-        <v>212754</v>
+        <v>219767</v>
       </c>
       <c r="E127">
-        <v>39352</v>
+        <v>51356</v>
       </c>
       <c r="F127" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>7.9370000000000003</v>
+        <v>11.483000000000001</v>
       </c>
       <c r="B128">
-        <v>7.78</v>
+        <v>11.41</v>
       </c>
       <c r="C128">
-        <v>8.4</v>
+        <v>11.657999999999999</v>
       </c>
       <c r="D128">
-        <v>192177</v>
+        <v>186856</v>
       </c>
       <c r="E128">
-        <v>25962</v>
+        <v>68811</v>
       </c>
       <c r="F128" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>10.173</v>
+        <v>12.44</v>
       </c>
       <c r="B129">
-        <v>10.071</v>
+        <v>12.385999999999999</v>
       </c>
       <c r="C129">
-        <v>10.449</v>
+        <v>12.61</v>
       </c>
       <c r="D129">
-        <v>219767</v>
+        <v>214558</v>
       </c>
       <c r="E129">
-        <v>51356</v>
+        <v>94596</v>
       </c>
       <c r="F129" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>11.483000000000001</v>
+        <v>13.207000000000001</v>
       </c>
       <c r="B130">
-        <v>11.41</v>
+        <v>13.16</v>
       </c>
       <c r="C130">
-        <v>11.657999999999999</v>
+        <v>13.319000000000001</v>
       </c>
       <c r="D130">
-        <v>186856</v>
+        <v>173541</v>
       </c>
       <c r="E130">
-        <v>68811</v>
+        <v>85396</v>
       </c>
       <c r="F130" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>12.44</v>
+        <v>13.858000000000001</v>
       </c>
       <c r="B131">
-        <v>12.385999999999999</v>
+        <v>13.808999999999999</v>
       </c>
       <c r="C131">
-        <v>12.61</v>
+        <v>13.949</v>
       </c>
       <c r="D131">
-        <v>214558</v>
+        <v>219545</v>
       </c>
       <c r="E131">
-        <v>94596</v>
+        <v>119240</v>
       </c>
       <c r="F131" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>13.207000000000001</v>
+        <v>14.432</v>
       </c>
       <c r="B132">
-        <v>13.16</v>
+        <v>14.397</v>
       </c>
       <c r="C132">
-        <v>13.319000000000001</v>
+        <v>14.518000000000001</v>
       </c>
       <c r="D132">
-        <v>173541</v>
+        <v>163779</v>
       </c>
       <c r="E132">
-        <v>85396</v>
+        <v>91552</v>
       </c>
       <c r="F132" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133">
-        <v>13.858000000000001</v>
-      </c>
-      <c r="B133">
-        <v>13.808999999999999</v>
-      </c>
-      <c r="C133">
-        <v>13.949</v>
-      </c>
-      <c r="D133">
-        <v>219545</v>
-      </c>
-      <c r="E133">
-        <v>119240</v>
+      <c r="A133" t="s">
+        <v>24</v>
+      </c>
+      <c r="B133" t="s">
+        <v>24</v>
+      </c>
+      <c r="C133" t="s">
+        <v>24</v>
+      </c>
+      <c r="D133" t="s">
+        <v>24</v>
+      </c>
+      <c r="E133" t="s">
+        <v>24</v>
       </c>
       <c r="F133" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>14.432</v>
+        <v>3.4489999999999998</v>
       </c>
       <c r="B134">
-        <v>14.397</v>
+        <v>3.355</v>
       </c>
       <c r="C134">
-        <v>14.518000000000001</v>
+        <v>3.6629999999999998</v>
       </c>
       <c r="D134">
-        <v>163779</v>
+        <v>162714</v>
       </c>
       <c r="E134">
-        <v>91552</v>
+        <v>36672</v>
       </c>
       <c r="F134" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>24</v>
-      </c>
-      <c r="B135" t="s">
-        <v>24</v>
-      </c>
-      <c r="C135" t="s">
-        <v>24</v>
-      </c>
-      <c r="D135" t="s">
-        <v>24</v>
-      </c>
-      <c r="E135" t="s">
-        <v>24</v>
+      <c r="A135">
+        <v>4.5679999999999996</v>
+      </c>
+      <c r="B135">
+        <v>4.4240000000000004</v>
+      </c>
+      <c r="C135">
+        <v>4.7830000000000004</v>
+      </c>
+      <c r="D135">
+        <v>200070</v>
+      </c>
+      <c r="E135">
+        <v>40766</v>
       </c>
       <c r="F135" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>3.4489999999999998</v>
+        <v>6.0049999999999999</v>
       </c>
       <c r="B136">
-        <v>3.355</v>
+        <v>5.9080000000000004</v>
       </c>
       <c r="C136">
-        <v>3.6629999999999998</v>
+        <v>6.2670000000000003</v>
       </c>
       <c r="D136">
-        <v>162714</v>
+        <v>210323</v>
       </c>
       <c r="E136">
-        <v>36672</v>
+        <v>39585</v>
       </c>
       <c r="F136" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>4.5679999999999996</v>
+        <v>7.9260000000000002</v>
       </c>
       <c r="B137">
-        <v>4.4240000000000004</v>
+        <v>7.77</v>
       </c>
       <c r="C137">
-        <v>4.7830000000000004</v>
+        <v>8.3949999999999996</v>
       </c>
       <c r="D137">
-        <v>200070</v>
+        <v>198363</v>
       </c>
       <c r="E137">
-        <v>40766</v>
+        <v>28641</v>
       </c>
       <c r="F137" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>6.0049999999999999</v>
+        <v>10.164999999999999</v>
       </c>
       <c r="B138">
-        <v>5.9080000000000004</v>
+        <v>10.066000000000001</v>
       </c>
       <c r="C138">
-        <v>6.2670000000000003</v>
+        <v>10.449</v>
       </c>
       <c r="D138">
-        <v>210323</v>
+        <v>211755</v>
       </c>
       <c r="E138">
-        <v>39585</v>
+        <v>50875</v>
       </c>
       <c r="F138" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>7.9260000000000002</v>
+        <v>11.478999999999999</v>
       </c>
       <c r="B139">
-        <v>7.77</v>
+        <v>11.414999999999999</v>
       </c>
       <c r="C139">
-        <v>8.3949999999999996</v>
+        <v>11.667</v>
       </c>
       <c r="D139">
-        <v>198363</v>
+        <v>193685</v>
       </c>
       <c r="E139">
-        <v>28641</v>
+        <v>68911</v>
       </c>
       <c r="F139" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>10.164999999999999</v>
+        <v>12.436999999999999</v>
       </c>
       <c r="B140">
-        <v>10.066000000000001</v>
+        <v>12.375999999999999</v>
       </c>
       <c r="C140">
-        <v>10.449</v>
+        <v>12.609</v>
       </c>
       <c r="D140">
-        <v>211755</v>
+        <v>206044</v>
       </c>
       <c r="E140">
-        <v>50875</v>
+        <v>91273</v>
       </c>
       <c r="F140" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>11.478999999999999</v>
+        <v>13.206</v>
       </c>
       <c r="B141">
-        <v>11.414999999999999</v>
+        <v>13.16</v>
       </c>
       <c r="C141">
-        <v>11.667</v>
+        <v>13.319000000000001</v>
       </c>
       <c r="D141">
-        <v>193685</v>
+        <v>180090</v>
       </c>
       <c r="E141">
-        <v>68911</v>
+        <v>86822</v>
       </c>
       <c r="F141" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>12.436999999999999</v>
+        <v>13.858000000000001</v>
       </c>
       <c r="B142">
-        <v>12.375999999999999</v>
+        <v>13.813000000000001</v>
       </c>
       <c r="C142">
-        <v>12.609</v>
+        <v>13.952999999999999</v>
       </c>
       <c r="D142">
-        <v>206044</v>
+        <v>212654</v>
       </c>
       <c r="E142">
-        <v>91273</v>
+        <v>115293</v>
       </c>
       <c r="F142" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>13.206</v>
+        <v>14.430999999999999</v>
       </c>
       <c r="B143">
-        <v>13.16</v>
+        <v>14.391999999999999</v>
       </c>
       <c r="C143">
-        <v>13.319000000000001</v>
+        <v>14.509</v>
       </c>
       <c r="D143">
-        <v>180090</v>
+        <v>172623</v>
       </c>
       <c r="E143">
-        <v>86822</v>
+        <v>97800</v>
       </c>
       <c r="F143" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <v>13.858000000000001</v>
-      </c>
-      <c r="B144">
-        <v>13.813000000000001</v>
-      </c>
-      <c r="C144">
-        <v>13.952999999999999</v>
-      </c>
-      <c r="D144">
-        <v>212654</v>
-      </c>
-      <c r="E144">
-        <v>115293</v>
+      <c r="A144" t="s">
+        <v>25</v>
+      </c>
+      <c r="B144" t="s">
+        <v>25</v>
+      </c>
+      <c r="C144" t="s">
+        <v>25</v>
+      </c>
+      <c r="D144" t="s">
+        <v>25</v>
+      </c>
+      <c r="E144" t="s">
+        <v>25</v>
       </c>
       <c r="F144" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>14.430999999999999</v>
+        <v>3.444</v>
       </c>
       <c r="B145">
-        <v>14.391999999999999</v>
+        <v>3.3650000000000002</v>
       </c>
       <c r="C145">
-        <v>14.509</v>
+        <v>3.6549999999999998</v>
       </c>
       <c r="D145">
-        <v>172623</v>
+        <v>131546</v>
       </c>
       <c r="E145">
-        <v>97800</v>
+        <v>31232</v>
       </c>
       <c r="F145" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>25</v>
-      </c>
-      <c r="B146" t="s">
-        <v>25</v>
-      </c>
-      <c r="C146" t="s">
-        <v>25</v>
-      </c>
-      <c r="D146" t="s">
-        <v>25</v>
-      </c>
-      <c r="E146" t="s">
-        <v>25</v>
+      <c r="A146">
+        <v>4.5640000000000001</v>
+      </c>
+      <c r="B146">
+        <v>4.4290000000000003</v>
+      </c>
+      <c r="C146">
+        <v>4.7839999999999998</v>
+      </c>
+      <c r="D146">
+        <v>167830</v>
+      </c>
+      <c r="E146">
+        <v>35261</v>
       </c>
       <c r="F146" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>3.444</v>
+        <v>5.9980000000000002</v>
       </c>
       <c r="B147">
-        <v>3.3650000000000002</v>
+        <v>5.9039999999999999</v>
       </c>
       <c r="C147">
-        <v>3.6549999999999998</v>
+        <v>6.2450000000000001</v>
       </c>
       <c r="D147">
-        <v>131546</v>
+        <v>177734</v>
       </c>
       <c r="E147">
-        <v>31232</v>
+        <v>34804</v>
       </c>
       <c r="F147" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>4.5640000000000001</v>
+        <v>7.9169999999999998</v>
       </c>
       <c r="B148">
-        <v>4.4290000000000003</v>
+        <v>7.7709999999999999</v>
       </c>
       <c r="C148">
-        <v>4.7839999999999998</v>
+        <v>8.3490000000000002</v>
       </c>
       <c r="D148">
-        <v>167830</v>
+        <v>181353</v>
       </c>
       <c r="E148">
-        <v>35261</v>
+        <v>27550</v>
       </c>
       <c r="F148" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>5.9980000000000002</v>
+        <v>10.157999999999999</v>
       </c>
       <c r="B149">
-        <v>5.9039999999999999</v>
+        <v>10.067</v>
       </c>
       <c r="C149">
-        <v>6.2450000000000001</v>
+        <v>10.426</v>
       </c>
       <c r="D149">
-        <v>177734</v>
+        <v>193641</v>
       </c>
       <c r="E149">
-        <v>34804</v>
+        <v>47095</v>
       </c>
       <c r="F149" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>7.9169999999999998</v>
+        <v>11.475</v>
       </c>
       <c r="B150">
-        <v>7.7709999999999999</v>
+        <v>11.406000000000001</v>
       </c>
       <c r="C150">
-        <v>8.3490000000000002</v>
+        <v>11.663</v>
       </c>
       <c r="D150">
-        <v>181353</v>
+        <v>194867</v>
       </c>
       <c r="E150">
-        <v>27550</v>
+        <v>69660</v>
       </c>
       <c r="F150" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>10.157999999999999</v>
+        <v>12.435</v>
       </c>
       <c r="B151">
-        <v>10.067</v>
+        <v>12.381</v>
       </c>
       <c r="C151">
-        <v>10.426</v>
+        <v>12.601000000000001</v>
       </c>
       <c r="D151">
-        <v>193641</v>
+        <v>194492</v>
       </c>
       <c r="E151">
-        <v>47095</v>
+        <v>86282</v>
       </c>
       <c r="F151" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>11.475</v>
+        <v>13.205</v>
       </c>
       <c r="B152">
-        <v>11.406000000000001</v>
+        <v>13.114000000000001</v>
       </c>
       <c r="C152">
-        <v>11.663</v>
+        <v>13.319000000000001</v>
       </c>
       <c r="D152">
-        <v>194867</v>
+        <v>190821</v>
       </c>
       <c r="E152">
-        <v>69660</v>
+        <v>95724</v>
       </c>
       <c r="F152" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>12.435</v>
+        <v>13.856999999999999</v>
       </c>
       <c r="B153">
-        <v>12.381</v>
+        <v>13.808999999999999</v>
       </c>
       <c r="C153">
-        <v>12.601000000000001</v>
+        <v>13.954000000000001</v>
       </c>
       <c r="D153">
-        <v>194492</v>
+        <v>202536</v>
       </c>
       <c r="E153">
-        <v>86282</v>
+        <v>108233</v>
       </c>
       <c r="F153" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>13.205</v>
+        <v>14.430999999999999</v>
       </c>
       <c r="B154">
-        <v>13.114000000000001</v>
+        <v>14.393000000000001</v>
       </c>
       <c r="C154">
-        <v>13.319000000000001</v>
+        <v>14.513999999999999</v>
       </c>
       <c r="D154">
-        <v>190821</v>
+        <v>185716</v>
       </c>
       <c r="E154">
-        <v>95724</v>
+        <v>103795</v>
       </c>
       <c r="F154" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155">
-        <v>13.856999999999999</v>
-      </c>
-      <c r="B155">
-        <v>13.808999999999999</v>
-      </c>
-      <c r="C155">
-        <v>13.954000000000001</v>
-      </c>
-      <c r="D155">
-        <v>202536</v>
-      </c>
-      <c r="E155">
-        <v>108233</v>
+      <c r="A155" t="s">
+        <v>26</v>
+      </c>
+      <c r="B155" t="s">
+        <v>26</v>
+      </c>
+      <c r="C155" t="s">
+        <v>26</v>
+      </c>
+      <c r="D155" t="s">
+        <v>26</v>
+      </c>
+      <c r="E155" t="s">
+        <v>26</v>
       </c>
       <c r="F155" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>14.430999999999999</v>
+        <v>3.4380000000000002</v>
       </c>
       <c r="B156">
-        <v>14.393000000000001</v>
+        <v>3.3650000000000002</v>
       </c>
       <c r="C156">
-        <v>14.513999999999999</v>
+        <v>3.645</v>
       </c>
       <c r="D156">
-        <v>185716</v>
+        <v>106907</v>
       </c>
       <c r="E156">
-        <v>103795</v>
+        <v>25838</v>
       </c>
       <c r="F156" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>26</v>
-      </c>
-      <c r="B157" t="s">
-        <v>26</v>
-      </c>
-      <c r="C157" t="s">
-        <v>26</v>
-      </c>
-      <c r="D157" t="s">
-        <v>26</v>
-      </c>
-      <c r="E157" t="s">
-        <v>26</v>
+      <c r="A157">
+        <v>5.9939999999999998</v>
+      </c>
+      <c r="B157">
+        <v>5.88</v>
+      </c>
+      <c r="C157">
+        <v>6.24</v>
+      </c>
+      <c r="D157">
+        <v>126880</v>
+      </c>
+      <c r="E157">
+        <v>26439</v>
       </c>
       <c r="F157" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>3.4380000000000002</v>
+        <v>10.154999999999999</v>
       </c>
       <c r="B158">
-        <v>3.3650000000000002</v>
+        <v>10.057</v>
       </c>
       <c r="C158">
-        <v>3.645</v>
+        <v>10.435</v>
       </c>
       <c r="D158">
-        <v>106907</v>
+        <v>130236</v>
       </c>
       <c r="E158">
-        <v>25838</v>
+        <v>32454</v>
       </c>
       <c r="F158" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>5.9939999999999998</v>
+        <v>12.436</v>
       </c>
       <c r="B159">
-        <v>5.88</v>
+        <v>12.381</v>
       </c>
       <c r="C159">
-        <v>6.24</v>
+        <v>12.61</v>
       </c>
       <c r="D159">
-        <v>126880</v>
+        <v>125522</v>
       </c>
       <c r="E159">
-        <v>26439</v>
+        <v>55950</v>
       </c>
       <c r="F159" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>10.154999999999999</v>
+        <v>13.859</v>
       </c>
       <c r="B160">
-        <v>10.057</v>
+        <v>13.804</v>
       </c>
       <c r="C160">
-        <v>10.435</v>
+        <v>14.01</v>
       </c>
       <c r="D160">
-        <v>130236</v>
+        <v>130941</v>
       </c>
       <c r="E160">
-        <v>32454</v>
+        <v>65271</v>
       </c>
       <c r="F160" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161">
-        <v>12.436</v>
-      </c>
-      <c r="B161">
-        <v>12.381</v>
-      </c>
-      <c r="C161">
-        <v>12.61</v>
-      </c>
-      <c r="D161">
-        <v>125522</v>
-      </c>
-      <c r="E161">
-        <v>55950</v>
+      <c r="A161" t="s">
+        <v>27</v>
+      </c>
+      <c r="B161" t="s">
+        <v>27</v>
+      </c>
+      <c r="C161" t="s">
+        <v>27</v>
+      </c>
+      <c r="D161" t="s">
+        <v>27</v>
+      </c>
+      <c r="E161" t="s">
+        <v>27</v>
       </c>
       <c r="F161" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>13.859</v>
+        <v>3.4540000000000002</v>
       </c>
       <c r="B162">
-        <v>13.804</v>
+        <v>3.37</v>
       </c>
       <c r="C162">
-        <v>14.01</v>
+        <v>3.6640000000000001</v>
       </c>
       <c r="D162">
-        <v>130941</v>
+        <v>155039</v>
       </c>
       <c r="E162">
-        <v>65271</v>
+        <v>34954</v>
       </c>
       <c r="F162" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>27</v>
-      </c>
-      <c r="B163" t="s">
-        <v>27</v>
-      </c>
-      <c r="C163" t="s">
-        <v>27</v>
-      </c>
-      <c r="D163" t="s">
-        <v>27</v>
-      </c>
-      <c r="E163" t="s">
-        <v>27</v>
+      <c r="A163">
+        <v>4.5780000000000003</v>
+      </c>
+      <c r="B163">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="C163">
+        <v>4.625</v>
+      </c>
+      <c r="D163">
+        <v>415</v>
+      </c>
+      <c r="E163">
+        <v>183</v>
       </c>
       <c r="F163" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>3.4540000000000002</v>
+        <v>4.681</v>
       </c>
       <c r="B164">
-        <v>3.37</v>
+        <v>4.625</v>
       </c>
       <c r="C164">
-        <v>3.6640000000000001</v>
+        <v>4.7229999999999999</v>
       </c>
       <c r="D164">
-        <v>155039</v>
+        <v>644</v>
       </c>
       <c r="E164">
-        <v>34954</v>
+        <v>166</v>
       </c>
       <c r="F164" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>4.5780000000000003</v>
+        <v>6.0149999999999997</v>
       </c>
       <c r="B165">
-        <v>4.5599999999999996</v>
+        <v>5.9219999999999997</v>
       </c>
       <c r="C165">
-        <v>4.625</v>
+        <v>6.2069999999999999</v>
       </c>
       <c r="D165">
-        <v>415</v>
+        <v>197266</v>
       </c>
       <c r="E165">
-        <v>183</v>
+        <v>37321</v>
       </c>
       <c r="F165" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>4.681</v>
+        <v>10.172000000000001</v>
       </c>
       <c r="B166">
-        <v>4.625</v>
+        <v>10.066000000000001</v>
       </c>
       <c r="C166">
-        <v>4.7229999999999999</v>
+        <v>10.462999999999999</v>
       </c>
       <c r="D166">
-        <v>644</v>
+        <v>192520</v>
       </c>
       <c r="E166">
-        <v>166</v>
+        <v>46192</v>
       </c>
       <c r="F166" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>6.0149999999999997</v>
+        <v>12.442</v>
       </c>
       <c r="B167">
-        <v>5.9219999999999997</v>
+        <v>12.381</v>
       </c>
       <c r="C167">
-        <v>6.2069999999999999</v>
+        <v>12.61</v>
       </c>
       <c r="D167">
-        <v>197266</v>
+        <v>183659</v>
       </c>
       <c r="E167">
-        <v>37321</v>
+        <v>81543</v>
       </c>
       <c r="F167" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>10.172000000000001</v>
+        <v>13.861000000000001</v>
       </c>
       <c r="B168">
-        <v>10.066000000000001</v>
+        <v>13.818</v>
       </c>
       <c r="C168">
-        <v>10.462999999999999</v>
+        <v>13.991</v>
       </c>
       <c r="D168">
-        <v>192520</v>
+        <v>189480</v>
       </c>
       <c r="E168">
-        <v>46192</v>
+        <v>100593</v>
       </c>
       <c r="F168" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169">
-        <v>12.442</v>
-      </c>
-      <c r="B169">
-        <v>12.381</v>
-      </c>
-      <c r="C169">
-        <v>12.61</v>
-      </c>
-      <c r="D169">
-        <v>183659</v>
-      </c>
-      <c r="E169">
-        <v>81543</v>
+      <c r="A169" t="s">
+        <v>28</v>
+      </c>
+      <c r="B169" t="s">
+        <v>28</v>
+      </c>
+      <c r="C169" t="s">
+        <v>28</v>
+      </c>
+      <c r="D169" t="s">
+        <v>28</v>
+      </c>
+      <c r="E169" t="s">
+        <v>28</v>
       </c>
       <c r="F169" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>13.861000000000001</v>
+        <v>3.4489999999999998</v>
       </c>
       <c r="B170">
-        <v>13.818</v>
+        <v>3.3559999999999999</v>
       </c>
       <c r="C170">
-        <v>13.991</v>
+        <v>3.6589999999999998</v>
       </c>
       <c r="D170">
-        <v>189480</v>
+        <v>171856</v>
       </c>
       <c r="E170">
-        <v>100593</v>
+        <v>40943</v>
       </c>
       <c r="F170" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>28</v>
-      </c>
-      <c r="B171" t="s">
-        <v>28</v>
-      </c>
-      <c r="C171" t="s">
-        <v>28</v>
-      </c>
-      <c r="D171" t="s">
-        <v>28</v>
-      </c>
-      <c r="E171" t="s">
-        <v>28</v>
+      <c r="A171">
+        <v>6.0030000000000001</v>
+      </c>
+      <c r="B171">
+        <v>5.899</v>
+      </c>
+      <c r="C171">
+        <v>6.4080000000000004</v>
+      </c>
+      <c r="D171">
+        <v>201164</v>
+      </c>
+      <c r="E171">
+        <v>39873</v>
       </c>
       <c r="F171" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>3.4489999999999998</v>
+        <v>10.162000000000001</v>
       </c>
       <c r="B172">
-        <v>3.3559999999999999</v>
+        <v>10.057</v>
       </c>
       <c r="C172">
-        <v>3.6589999999999998</v>
+        <v>10.454000000000001</v>
       </c>
       <c r="D172">
-        <v>171856</v>
+        <v>199497</v>
       </c>
       <c r="E172">
-        <v>40943</v>
+        <v>49588</v>
       </c>
       <c r="F172" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>6.0030000000000001</v>
+        <v>12.439</v>
       </c>
       <c r="B173">
-        <v>5.899</v>
+        <v>12.377000000000001</v>
       </c>
       <c r="C173">
-        <v>6.4080000000000004</v>
+        <v>12.61</v>
       </c>
       <c r="D173">
-        <v>201164</v>
+        <v>182108</v>
       </c>
       <c r="E173">
-        <v>39873</v>
+        <v>80583</v>
       </c>
       <c r="F173" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>10.162000000000001</v>
+        <v>13.86</v>
       </c>
       <c r="B174">
-        <v>10.057</v>
+        <v>13.819000000000001</v>
       </c>
       <c r="C174">
-        <v>10.454000000000001</v>
+        <v>13.973000000000001</v>
       </c>
       <c r="D174">
-        <v>199497</v>
+        <v>179919</v>
       </c>
       <c r="E174">
-        <v>49588</v>
+        <v>93889</v>
       </c>
       <c r="F174" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>12.439</v>
+        <v>14.349</v>
       </c>
       <c r="B175">
-        <v>12.377000000000001</v>
+        <v>14.323</v>
       </c>
       <c r="C175">
-        <v>12.61</v>
+        <v>14.388</v>
       </c>
       <c r="D175">
-        <v>182108</v>
+        <v>2115</v>
       </c>
       <c r="E175">
-        <v>80583</v>
+        <v>1239</v>
       </c>
       <c r="F175" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176">
-        <v>13.86</v>
-      </c>
-      <c r="B176">
-        <v>13.819000000000001</v>
-      </c>
-      <c r="C176">
-        <v>13.973000000000001</v>
-      </c>
-      <c r="D176">
-        <v>179919</v>
-      </c>
-      <c r="E176">
-        <v>93889</v>
+      <c r="A176" t="s">
+        <v>29</v>
+      </c>
+      <c r="B176" t="s">
+        <v>29</v>
+      </c>
+      <c r="C176" t="s">
+        <v>29</v>
+      </c>
+      <c r="D176" t="s">
+        <v>29</v>
+      </c>
+      <c r="E176" t="s">
+        <v>29</v>
       </c>
       <c r="F176" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>14.349</v>
+        <v>3.4550000000000001</v>
       </c>
       <c r="B177">
-        <v>14.323</v>
+        <v>3.3740000000000001</v>
       </c>
       <c r="C177">
-        <v>14.388</v>
+        <v>3.6539999999999999</v>
       </c>
       <c r="D177">
-        <v>2115</v>
+        <v>163222</v>
       </c>
       <c r="E177">
-        <v>1239</v>
+        <v>37025</v>
       </c>
       <c r="F177" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>29</v>
-      </c>
-      <c r="B178" t="s">
-        <v>29</v>
-      </c>
-      <c r="C178" t="s">
-        <v>29</v>
-      </c>
-      <c r="D178" t="s">
-        <v>29</v>
-      </c>
-      <c r="E178" t="s">
-        <v>29</v>
+      <c r="A178">
+        <v>4.5789999999999997</v>
+      </c>
+      <c r="B178">
+        <v>4.452</v>
+      </c>
+      <c r="C178">
+        <v>4.8070000000000004</v>
+      </c>
+      <c r="D178">
+        <v>726092</v>
+      </c>
+      <c r="E178">
+        <v>148680</v>
       </c>
       <c r="F178" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>3.4550000000000001</v>
+        <v>6.0129999999999999</v>
       </c>
       <c r="B179">
-        <v>3.3740000000000001</v>
+        <v>5.9180000000000001</v>
       </c>
       <c r="C179">
-        <v>3.6539999999999999</v>
+        <v>6.2859999999999996</v>
       </c>
       <c r="D179">
-        <v>163222</v>
+        <v>210846</v>
       </c>
       <c r="E179">
-        <v>37025</v>
+        <v>38791</v>
       </c>
       <c r="F179" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>4.5789999999999997</v>
+        <v>7.9779999999999998</v>
       </c>
       <c r="B180">
-        <v>4.452</v>
+        <v>7.78</v>
       </c>
       <c r="C180">
-        <v>4.8070000000000004</v>
+        <v>8.5030000000000001</v>
       </c>
       <c r="D180">
-        <v>726092</v>
+        <v>2602373</v>
       </c>
       <c r="E180">
-        <v>148680</v>
+        <v>367231</v>
       </c>
       <c r="F180" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>6.0129999999999999</v>
+        <v>10.173999999999999</v>
       </c>
       <c r="B181">
-        <v>5.9180000000000001</v>
+        <v>10.023999999999999</v>
       </c>
       <c r="C181">
-        <v>6.2859999999999996</v>
+        <v>10.412000000000001</v>
       </c>
       <c r="D181">
-        <v>210846</v>
+        <v>211112</v>
       </c>
       <c r="E181">
-        <v>38791</v>
+        <v>50266</v>
       </c>
       <c r="F181" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>7.9779999999999998</v>
+        <v>11.525</v>
       </c>
       <c r="B182">
-        <v>7.78</v>
+        <v>11.414999999999999</v>
       </c>
       <c r="C182">
-        <v>8.5030000000000001</v>
+        <v>11.662000000000001</v>
       </c>
       <c r="D182">
-        <v>2602373</v>
+        <v>3431965</v>
       </c>
       <c r="E182">
-        <v>367231</v>
+        <v>1051299</v>
       </c>
       <c r="F182" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>10.173999999999999</v>
+        <v>12.441000000000001</v>
       </c>
       <c r="B183">
-        <v>10.023999999999999</v>
+        <v>12.381</v>
       </c>
       <c r="C183">
-        <v>10.412000000000001</v>
+        <v>12.577</v>
       </c>
       <c r="D183">
-        <v>211112</v>
+        <v>203716</v>
       </c>
       <c r="E183">
-        <v>50266</v>
+        <v>87985</v>
       </c>
       <c r="F183" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>11.525</v>
+        <v>13.233000000000001</v>
       </c>
       <c r="B184">
-        <v>11.414999999999999</v>
+        <v>13.16</v>
       </c>
       <c r="C184">
-        <v>11.662000000000001</v>
+        <v>13.337999999999999</v>
       </c>
       <c r="D184">
-        <v>3431965</v>
+        <v>2171436</v>
       </c>
       <c r="E184">
-        <v>1051299</v>
+        <v>958860</v>
       </c>
       <c r="F184" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>12.441000000000001</v>
+        <v>13.86</v>
       </c>
       <c r="B185">
-        <v>12.381</v>
+        <v>13.823</v>
       </c>
       <c r="C185">
-        <v>12.577</v>
+        <v>13.962999999999999</v>
       </c>
       <c r="D185">
-        <v>203716</v>
+        <v>217729</v>
       </c>
       <c r="E185">
-        <v>87985</v>
+        <v>112506</v>
       </c>
       <c r="F185" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>13.233000000000001</v>
+        <v>14.436999999999999</v>
       </c>
       <c r="B186">
-        <v>13.16</v>
+        <v>14.397</v>
       </c>
       <c r="C186">
-        <v>13.337999999999999</v>
+        <v>14.523</v>
       </c>
       <c r="D186">
-        <v>2171436</v>
+        <v>407922</v>
       </c>
       <c r="E186">
-        <v>958860</v>
+        <v>233256</v>
       </c>
       <c r="F186" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A187">
-        <v>13.86</v>
-      </c>
-      <c r="B187">
-        <v>13.823</v>
-      </c>
-      <c r="C187">
-        <v>13.962999999999999</v>
-      </c>
-      <c r="D187">
-        <v>217729</v>
-      </c>
-      <c r="E187">
-        <v>112506</v>
+      <c r="A187" t="s">
+        <v>30</v>
+      </c>
+      <c r="B187" t="s">
+        <v>30</v>
+      </c>
+      <c r="C187" t="s">
+        <v>30</v>
+      </c>
+      <c r="D187" t="s">
+        <v>30</v>
+      </c>
+      <c r="E187" t="s">
+        <v>30</v>
       </c>
       <c r="F187" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>14.318</v>
+        <v>3.4329999999999998</v>
       </c>
       <c r="B188">
-        <v>14.243</v>
+        <v>3.3559999999999999</v>
       </c>
       <c r="C188">
-        <v>14.340999999999999</v>
+        <v>3.6309999999999998</v>
       </c>
       <c r="D188">
-        <v>1559</v>
+        <v>108413</v>
       </c>
       <c r="E188">
-        <v>405</v>
+        <v>26712</v>
       </c>
       <c r="F188" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>14.436999999999999</v>
+        <v>5.9870000000000001</v>
       </c>
       <c r="B189">
-        <v>14.397</v>
+        <v>5.89</v>
       </c>
       <c r="C189">
-        <v>14.523</v>
+        <v>6.1980000000000004</v>
       </c>
       <c r="D189">
-        <v>407922</v>
+        <v>117770</v>
       </c>
       <c r="E189">
-        <v>233256</v>
+        <v>24954</v>
       </c>
       <c r="F189" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>30</v>
-      </c>
-      <c r="B190" t="s">
-        <v>30</v>
-      </c>
-      <c r="C190" t="s">
-        <v>30</v>
-      </c>
-      <c r="D190" t="s">
-        <v>30</v>
-      </c>
-      <c r="E190" t="s">
-        <v>30</v>
+      <c r="A190">
+        <v>7.9210000000000003</v>
+      </c>
+      <c r="B190">
+        <v>7.7519999999999998</v>
+      </c>
+      <c r="C190">
+        <v>8.6850000000000005</v>
+      </c>
+      <c r="D190">
+        <v>1157917</v>
+      </c>
+      <c r="E190">
+        <v>196312</v>
       </c>
       <c r="F190" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>3.4329999999999998</v>
+        <v>10.147</v>
       </c>
       <c r="B191">
-        <v>3.3559999999999999</v>
+        <v>10.061999999999999</v>
       </c>
       <c r="C191">
-        <v>3.6309999999999998</v>
+        <v>10.388</v>
       </c>
       <c r="D191">
-        <v>108413</v>
+        <v>113969</v>
       </c>
       <c r="E191">
-        <v>26712</v>
+        <v>28666</v>
       </c>
       <c r="F191" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>5.9870000000000001</v>
+        <v>11.492000000000001</v>
       </c>
       <c r="B192">
-        <v>5.89</v>
+        <v>11.396000000000001</v>
       </c>
       <c r="C192">
-        <v>6.1980000000000004</v>
+        <v>11.662000000000001</v>
       </c>
       <c r="D192">
-        <v>117770</v>
+        <v>1478297</v>
       </c>
       <c r="E192">
-        <v>24954</v>
+        <v>526604</v>
       </c>
       <c r="F192" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>7.9210000000000003</v>
+        <v>12.433</v>
       </c>
       <c r="B193">
-        <v>7.7519999999999998</v>
+        <v>12.385999999999999</v>
       </c>
       <c r="C193">
-        <v>8.6850000000000005</v>
+        <v>12.571999999999999</v>
       </c>
       <c r="D193">
-        <v>1157917</v>
+        <v>108971</v>
       </c>
       <c r="E193">
-        <v>196312</v>
+        <v>48250</v>
       </c>
       <c r="F193" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>10.147</v>
+        <v>13.215999999999999</v>
       </c>
       <c r="B194">
-        <v>10.061999999999999</v>
+        <v>13.156000000000001</v>
       </c>
       <c r="C194">
-        <v>10.388</v>
+        <v>13.333</v>
       </c>
       <c r="D194">
-        <v>113969</v>
+        <v>941322</v>
       </c>
       <c r="E194">
-        <v>28666</v>
+        <v>451132</v>
       </c>
       <c r="F194" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>11.492000000000001</v>
+        <v>13.856999999999999</v>
       </c>
       <c r="B195">
-        <v>11.396000000000001</v>
+        <v>13.818</v>
       </c>
       <c r="C195">
-        <v>11.662000000000001</v>
+        <v>13.962999999999999</v>
       </c>
       <c r="D195">
-        <v>1478297</v>
+        <v>113009</v>
       </c>
       <c r="E195">
-        <v>526604</v>
+        <v>61128</v>
       </c>
       <c r="F195" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>12.433</v>
+        <v>14.433</v>
       </c>
       <c r="B196">
-        <v>12.385999999999999</v>
+        <v>14.397</v>
       </c>
       <c r="C196">
-        <v>12.571999999999999</v>
+        <v>14.523</v>
       </c>
       <c r="D196">
-        <v>108971</v>
+        <v>180396</v>
       </c>
       <c r="E196">
-        <v>48250</v>
+        <v>101573</v>
       </c>
       <c r="F196" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197">
-        <v>13.215999999999999</v>
-      </c>
-      <c r="B197">
-        <v>13.156000000000001</v>
-      </c>
-      <c r="C197">
-        <v>13.333</v>
-      </c>
-      <c r="D197">
-        <v>941322</v>
-      </c>
-      <c r="E197">
-        <v>451132</v>
+      <c r="A197" t="s">
+        <v>31</v>
+      </c>
+      <c r="B197" t="s">
+        <v>31</v>
+      </c>
+      <c r="C197" t="s">
+        <v>31</v>
+      </c>
+      <c r="D197" t="s">
+        <v>31</v>
+      </c>
+      <c r="E197" t="s">
+        <v>31</v>
       </c>
       <c r="F197" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>13.856999999999999</v>
+        <v>3.4569999999999999</v>
       </c>
       <c r="B198">
-        <v>13.818</v>
+        <v>3.3</v>
       </c>
       <c r="C198">
-        <v>13.962999999999999</v>
+        <v>3.673</v>
       </c>
       <c r="D198">
-        <v>113009</v>
+        <v>188787</v>
       </c>
       <c r="E198">
-        <v>61128</v>
+        <v>41877</v>
       </c>
       <c r="F198" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>14.318</v>
+        <v>4.5739999999999998</v>
       </c>
       <c r="B199">
-        <v>14.238</v>
+        <v>4.42</v>
       </c>
       <c r="C199">
-        <v>14.336</v>
+        <v>4.798</v>
       </c>
       <c r="D199">
-        <v>588</v>
+        <v>15782</v>
       </c>
       <c r="E199">
-        <v>159</v>
+        <v>2869</v>
       </c>
       <c r="F199" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>14.433</v>
+        <v>6.0129999999999999</v>
       </c>
       <c r="B200">
-        <v>14.397</v>
+        <v>5.9219999999999997</v>
       </c>
       <c r="C200">
-        <v>14.523</v>
+        <v>6.2770000000000001</v>
       </c>
       <c r="D200">
-        <v>180396</v>
+        <v>253048</v>
       </c>
       <c r="E200">
-        <v>101573</v>
+        <v>48149</v>
       </c>
       <c r="F200" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>31</v>
-      </c>
-      <c r="B201" t="s">
-        <v>31</v>
-      </c>
-      <c r="C201" t="s">
-        <v>31</v>
-      </c>
-      <c r="D201" t="s">
-        <v>31</v>
-      </c>
-      <c r="E201" t="s">
-        <v>31</v>
+      <c r="A201">
+        <v>7.9329999999999998</v>
+      </c>
+      <c r="B201">
+        <v>7.7889999999999997</v>
+      </c>
+      <c r="C201">
+        <v>8.1809999999999992</v>
+      </c>
+      <c r="D201">
+        <v>39957</v>
+      </c>
+      <c r="E201">
+        <v>5601</v>
       </c>
       <c r="F201" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>3.4569999999999999</v>
+        <v>10.172000000000001</v>
       </c>
       <c r="B202">
-        <v>3.3</v>
+        <v>10.066000000000001</v>
       </c>
       <c r="C202">
-        <v>3.673</v>
+        <v>10.416</v>
       </c>
       <c r="D202">
-        <v>188787</v>
+        <v>263936</v>
       </c>
       <c r="E202">
-        <v>41877</v>
+        <v>62788</v>
       </c>
       <c r="F202" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>4.5739999999999998</v>
+        <v>11.48</v>
       </c>
       <c r="B203">
-        <v>4.42</v>
+        <v>11.387</v>
       </c>
       <c r="C203">
-        <v>4.798</v>
+        <v>11.63</v>
       </c>
       <c r="D203">
-        <v>15782</v>
+        <v>54176</v>
       </c>
       <c r="E203">
-        <v>2869</v>
+        <v>19398</v>
       </c>
       <c r="F203" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>6.0129999999999999</v>
+        <v>12.44</v>
       </c>
       <c r="B204">
-        <v>5.9219999999999997</v>
+        <v>12.381</v>
       </c>
       <c r="C204">
-        <v>6.2770000000000001</v>
+        <v>12.577</v>
       </c>
       <c r="D204">
-        <v>253048</v>
+        <v>227608</v>
       </c>
       <c r="E204">
-        <v>48149</v>
+        <v>102253</v>
       </c>
       <c r="F204" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>7.9329999999999998</v>
+        <v>13.205</v>
       </c>
       <c r="B205">
-        <v>7.7889999999999997</v>
+        <v>13.16</v>
       </c>
       <c r="C205">
-        <v>8.1809999999999992</v>
+        <v>13.305</v>
       </c>
       <c r="D205">
-        <v>39957</v>
+        <v>33394</v>
       </c>
       <c r="E205">
-        <v>5601</v>
+        <v>16501</v>
       </c>
       <c r="F205" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>10.172000000000001</v>
+        <v>13.859</v>
       </c>
       <c r="B206">
-        <v>10.066000000000001</v>
+        <v>13.818</v>
       </c>
       <c r="C206">
-        <v>10.416</v>
+        <v>13.962999999999999</v>
       </c>
       <c r="D206">
-        <v>263936</v>
+        <v>209316</v>
       </c>
       <c r="E206">
-        <v>62788</v>
+        <v>112921</v>
       </c>
       <c r="F206" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>11.48</v>
+        <v>14.346</v>
       </c>
       <c r="B207">
-        <v>11.387</v>
+        <v>14.318</v>
       </c>
       <c r="C207">
-        <v>11.63</v>
+        <v>14.397</v>
       </c>
       <c r="D207">
-        <v>54176</v>
+        <v>8332</v>
       </c>
       <c r="E207">
-        <v>19398</v>
+        <v>4726</v>
       </c>
       <c r="F207" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A208">
-        <v>12.44</v>
-      </c>
-      <c r="B208">
-        <v>12.381</v>
-      </c>
-      <c r="C208">
-        <v>12.577</v>
-      </c>
-      <c r="D208">
-        <v>227608</v>
-      </c>
-      <c r="E208">
-        <v>102253</v>
-      </c>
-      <c r="F208" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A209">
-        <v>13.205</v>
-      </c>
-      <c r="B209">
-        <v>13.16</v>
-      </c>
-      <c r="C209">
-        <v>13.305</v>
-      </c>
-      <c r="D209">
-        <v>33394</v>
-      </c>
-      <c r="E209">
-        <v>16501</v>
-      </c>
-      <c r="F209" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A210">
-        <v>13.859</v>
-      </c>
-      <c r="B210">
-        <v>13.818</v>
-      </c>
-      <c r="C210">
-        <v>13.962999999999999</v>
-      </c>
-      <c r="D210">
-        <v>209316</v>
-      </c>
-      <c r="E210">
-        <v>112921</v>
-      </c>
-      <c r="F210" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A211">
-        <v>14.346</v>
-      </c>
-      <c r="B211">
-        <v>14.318</v>
-      </c>
-      <c r="C211">
-        <v>14.397</v>
-      </c>
-      <c r="D211">
-        <v>8332</v>
-      </c>
-      <c r="E211">
-        <v>4726</v>
-      </c>
-      <c r="F211" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212">
-        <v>14.429</v>
-      </c>
-      <c r="B212">
-        <v>14.397</v>
-      </c>
-      <c r="C212">
-        <v>14.476000000000001</v>
-      </c>
-      <c r="D212">
-        <v>6730</v>
-      </c>
-      <c r="E212">
-        <v>3560</v>
-      </c>
-      <c r="F212" t="s">
         <v>38</v>
       </c>
     </row>
@@ -43513,7 +43413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z211"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A148" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>

</xml_diff>